<commit_message>
Reorganisation of the tasks and time planning
</commit_message>
<xml_diff>
--- a/Gantt.xlsx
+++ b/Gantt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Escola\3. Uni\Curs 2020-2021\2n quatrimestre\TFG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07557B2E-F06C-4A28-9A58-4FB476DB138C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{282F237D-7359-4BD8-8100-DABE55C180E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{98C41FDD-CB4E-4972-98A2-CC4C313ED58E}"/>
   </bookViews>
@@ -33,25 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Standard play-by-play -&gt; Box score</t>
-  </si>
-  <si>
-    <t>Adaption to Basketball Reference data format</t>
-  </si>
-  <si>
-    <t>Full process design and correction and revision of possible errors</t>
-  </si>
-  <si>
-    <t>Interval-defined box score implementation</t>
-  </si>
-  <si>
-    <t>Design of information formats, such as graphics or tables</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Interface design</t>
   </si>
@@ -62,15 +44,6 @@
     <t>Memory completion</t>
   </si>
   <si>
-    <t>Implementation of a more sophisticated box score</t>
-  </si>
-  <si>
-    <t>Study of possible variables to be added</t>
-  </si>
-  <si>
-    <t>Basketball Reference play-by-play -&gt; Standard play-by-play</t>
-  </si>
-  <si>
     <t>Exploration of an advanced method for play recognition</t>
   </si>
   <si>
@@ -126,6 +99,15 @@
   </si>
   <si>
     <t>07/06-13/06</t>
+  </si>
+  <si>
+    <t>Advanced box score obtention</t>
+  </si>
+  <si>
+    <t>Simple box score obtention</t>
+  </si>
+  <si>
+    <t>Design of other match statistics supports</t>
   </si>
 </sst>
 </file>
@@ -167,7 +149,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -176,16 +158,78 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -194,10 +238,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -210,21 +253,28 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -539,172 +589,234 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6307673-B72C-43E5-93F0-C11225F59026}">
-  <dimension ref="A2:R24"/>
+  <dimension ref="A2:R19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" zoomScale="72" zoomScaleNormal="72" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="55" customWidth="1"/>
-    <col min="2" max="18" width="10.90625" customWidth="1"/>
+    <col min="1" max="1" width="45.7265625" customWidth="1"/>
+    <col min="2" max="18" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="L2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="M2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="N2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="O2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="P2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="Q2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="R2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="6" t="s">
+    </row>
+    <row r="3" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="14"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="12"/>
+      <c r="R3" s="12"/>
+    </row>
+    <row r="4" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="L2" s="5" t="s">
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
+      <c r="R4" s="12"/>
+    </row>
+    <row r="5" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="M2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q2" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="R2" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A3" s="8" t="s">
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="12"/>
+      <c r="R5" s="12"/>
+    </row>
+    <row r="6" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="14"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A4" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="14"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A5" s="10" t="s">
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="12"/>
+      <c r="R6" s="12"/>
+    </row>
+    <row r="7" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="12"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="12"/>
+      <c r="R7" s="12"/>
+    </row>
+    <row r="8" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="16"/>
+      <c r="Q8" s="12"/>
+      <c r="R8" s="12"/>
+    </row>
+    <row r="9" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="14"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A6" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A7" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="14"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A8" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A9" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A10" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="12"/>
+      <c r="P9" s="12"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="16"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A11" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A12" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="J12" s="2"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A13" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
-      <c r="P13" s="14"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A14" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q14" s="14"/>
-      <c r="R14" s="14"/>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="C16" s="1"/>
-    </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
+      <c r="C11" s="1"/>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>